<commit_message>
last notes :) wow, such a good feeling
</commit_message>
<xml_diff>
--- a/1.1-CS-4365.002-AI/Grades.xlsx
+++ b/1.1-CS-4365.002-AI/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDFall2018\1.1-CS-4365.002-AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076A88F7-C24F-46B4-A025-08E27F407932}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A95FF1B-E529-4279-9D8D-3728D193BFE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6630" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,16 +793,16 @@
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
-        <v>0.19800000000000001</v>
+        <v>0.24899999999999997</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="1"/>
-        <v>0.18000000000000002</v>
+        <v>0.124</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="23">
         <f>SUM(C7:H7)</f>
-        <v>0.60650000000000004</v>
+        <v>0.60150000000000003</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="5"/>
@@ -820,10 +820,10 @@
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="10">
-        <v>0.66</v>
+        <v>0.83</v>
       </c>
       <c r="H8" s="10">
-        <v>0.45</v>
+        <v>0.31</v>
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>

</xml_diff>

<commit_message>
Final Review for AI
</commit_message>
<xml_diff>
--- a/1.1-CS-4365.002-AI/Grades.xlsx
+++ b/1.1-CS-4365.002-AI/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDFall2018\1.1-CS-4365.002-AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A95FF1B-E529-4279-9D8D-3728D193BFE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B63390D-C75D-42F2-97F3-B47E9B3DA68C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6630" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,12 +797,12 @@
       </c>
       <c r="H7" s="9">
         <f t="shared" si="1"/>
-        <v>0.124</v>
+        <v>0.28399999999999997</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="23">
         <f>SUM(C7:H7)</f>
-        <v>0.60150000000000003</v>
+        <v>0.76150000000000007</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="5"/>
@@ -823,7 +823,7 @@
         <v>0.83</v>
       </c>
       <c r="H8" s="10">
-        <v>0.31</v>
+        <v>0.71</v>
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>

</xml_diff>

<commit_message>
Final commit, grades returned
</commit_message>
<xml_diff>
--- a/1.1-CS-4365.002-AI/Grades.xlsx
+++ b/1.1-CS-4365.002-AI/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDFall2018\1.1-CS-4365.002-AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B63390D-C75D-42F2-97F3-B47E9B3DA68C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D133F970-8A2F-4596-91BE-2B0361493C51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6630" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>4.3500000000000004E-2</v>
+        <v>6.4250000000000015E-2</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
@@ -797,12 +797,12 @@
       </c>
       <c r="H7" s="9">
         <f t="shared" si="1"/>
-        <v>0.28399999999999997</v>
+        <v>0.31400000000000006</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="23">
         <f>SUM(C7:H7)</f>
-        <v>0.76150000000000007</v>
+        <v>0.81225000000000003</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="5"/>
@@ -823,7 +823,7 @@
         <v>0.83</v>
       </c>
       <c r="H8" s="10">
-        <v>0.71</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
@@ -855,7 +855,7 @@
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="19">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="21"/>

</xml_diff>